<commit_message>
dynamic ability modifiers (model + dao)
</commit_message>
<xml_diff>
--- a/references/sketch.xlsx
+++ b/references/sketch.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="374">
   <si>
     <t>HP</t>
   </si>
@@ -1085,13 +1085,70 @@
   </si>
   <si>
     <t>critDmg</t>
+  </si>
+  <si>
+    <t>ability</t>
+  </si>
+  <si>
+    <t>mult</t>
+  </si>
+  <si>
+    <t>melee, composite bow</t>
+  </si>
+  <si>
+    <t>two handed + feat</t>
+  </si>
+  <si>
+    <t>improved weapon finesse</t>
+  </si>
+  <si>
+    <t>ranged, weapon finesse</t>
+  </si>
+  <si>
+    <t>ranged + zen archery</t>
+  </si>
+  <si>
+    <t>melee + two handed</t>
+  </si>
+  <si>
+    <t>melee + light</t>
+  </si>
+  <si>
+    <t>monk</t>
+  </si>
+  <si>
+    <t>standard</t>
+  </si>
+  <si>
+    <t>http://www.giantitp.com/forums/showthread.php?125732-3-x-X-stat-to-Y-bonus</t>
+  </si>
+  <si>
+    <t>fort</t>
+  </si>
+  <si>
+    <t>refl</t>
+  </si>
+  <si>
+    <t>skill</t>
+  </si>
+  <si>
+    <t>initiative</t>
+  </si>
+  <si>
+    <t>saves</t>
+  </si>
+  <si>
+    <t>hit</t>
+  </si>
+  <si>
+    <t>HP*lvl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1127,8 +1184,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1183,6 +1248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1202,10 +1273,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1248,12 +1320,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -3729,10 +3811,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3745,15 +3827,18 @@
     <col min="7" max="7" width="8.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>192</v>
       </c>
       <c r="C1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N1" s="23" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>297</v>
       </c>
@@ -3765,8 +3850,18 @@
       </c>
       <c r="F2" s="19"/>
       <c r="G2" s="19"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N2" s="19" t="s">
+        <v>355</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>356</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q2" s="19"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>298</v>
       </c>
@@ -3785,8 +3880,20 @@
       <c r="G3" s="19" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N3" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="24" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q3" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>300</v>
       </c>
@@ -3805,8 +3912,20 @@
       <c r="G4" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N4" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O4" s="24">
+        <v>1</v>
+      </c>
+      <c r="P4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="24" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>307</v>
       </c>
@@ -3825,8 +3944,18 @@
       <c r="G5" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N5" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="24">
+        <v>1</v>
+      </c>
+      <c r="P5" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q5" s="24"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>306</v>
       </c>
@@ -3845,8 +3974,18 @@
       <c r="G6" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="24">
+        <v>1</v>
+      </c>
+      <c r="P6" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q6" s="24"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>310</v>
       </c>
@@ -3856,8 +3995,18 @@
       <c r="C7" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N7" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O7" s="24">
+        <v>1</v>
+      </c>
+      <c r="P7" s="24" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q7" s="24"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>301</v>
       </c>
@@ -3872,8 +4021,18 @@
       </c>
       <c r="F8" s="19"/>
       <c r="G8" s="19"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
+      <c r="P8" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q8" s="24"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>302</v>
       </c>
@@ -3892,8 +4051,18 @@
       <c r="G9" s="19" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N9" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
+      <c r="P9" s="24" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q9" s="24"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>296</v>
       </c>
@@ -3912,8 +4081,20 @@
       <c r="G10" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>303</v>
       </c>
@@ -3932,8 +4113,20 @@
       <c r="G11" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N11" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="O11">
+        <v>1</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>304</v>
       </c>
@@ -3952,8 +4145,20 @@
       <c r="G12" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N12" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" s="22">
+        <v>0.5</v>
+      </c>
+      <c r="P12" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>305</v>
       </c>
@@ -3972,8 +4177,20 @@
       <c r="G13" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N13" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="22">
+        <v>1</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>156</v>
       </c>
@@ -3992,8 +4209,20 @@
       <c r="G14" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N14" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>336</v>
       </c>
@@ -4006,20 +4235,56 @@
       <c r="G15" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="N15" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="17" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="N16" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q16" s="22" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="17" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E17" s="19" t="s">
         <v>305</v>
       </c>
       <c r="F17" s="19"/>
       <c r="G17" s="19"/>
-    </row>
-    <row r="18" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="N17" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="O17">
+        <v>1</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q17" s="22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E18" s="19" t="s">
         <v>331</v>
       </c>
@@ -4029,8 +4294,20 @@
       <c r="G18" s="19" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="19" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="N18" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+      <c r="P18" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q18" s="22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="19" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E19">
         <v>1</v>
       </c>
@@ -4040,8 +4317,11 @@
       <c r="G19" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="20" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P19" s="22" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="20" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E20">
         <v>2</v>
       </c>
@@ -4051,8 +4331,11 @@
       <c r="G20" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="21" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P20" s="22" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="21" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E21">
         <v>3</v>
       </c>
@@ -4062,8 +4345,11 @@
       <c r="G21" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="22" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P21" s="22" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="22" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E22">
         <v>4</v>
       </c>
@@ -4073,8 +4359,11 @@
       <c r="G22" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="23" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P22" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="23" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E23">
         <v>5</v>
       </c>
@@ -4084,8 +4373,16 @@
       <c r="G23" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="25" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P23" s="22" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="24" spans="5:17" x14ac:dyDescent="0.25">
+      <c r="P24" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E25" s="19" t="s">
         <v>339</v>
       </c>
@@ -4096,8 +4393,11 @@
       <c r="J25" s="19"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
-    </row>
-    <row r="26" spans="5:12" x14ac:dyDescent="0.25">
+      <c r="P25" s="22" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="26" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E26" s="19" t="s">
         <v>331</v>
       </c>
@@ -4123,7 +4423,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="27" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="5:17" x14ac:dyDescent="0.25">
       <c r="E27">
         <v>1</v>
       </c>
@@ -4143,27 +4443,27 @@
         <v>347</v>
       </c>
     </row>
-    <row r="28" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="5:17" x14ac:dyDescent="0.25">
       <c r="H28" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="29" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="5:17" x14ac:dyDescent="0.25">
       <c r="H29" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="30" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="5:17" x14ac:dyDescent="0.25">
       <c r="H30" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="31" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="5:17" x14ac:dyDescent="0.25">
       <c r="H31" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="32" spans="5:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="5:17" x14ac:dyDescent="0.25">
       <c r="H32" t="s">
         <v>344</v>
       </c>
@@ -4209,7 +4509,10 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N1" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>